<commit_message>
Successfull program run + new test names for renaming
</commit_message>
<xml_diff>
--- a/_01_main/_02_tests/LibMan_renaming_test_names.xlsx
+++ b/_01_main/_02_tests/LibMan_renaming_test_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davis\00_data\01_Projects\Personal\SCDL\_01_main\_02_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A9FB5-6FD5-48D0-8264-E2A8AFBCE2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0722813C-B204-411E-BAD3-E618CC19EB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12720" xr2:uid="{9664D8D8-E09F-4482-9132-8996544CFBDA}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15555" xr2:uid="{9664D8D8-E09F-4482-9132-8996544CFBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>𝐏𝐑𝐄𝐌𝐈𝐄𝐑𝐄| [TFT Records] Illiam Patrol - With My Fist [TFT004]</t>
   </si>
@@ -126,6 +126,24 @@
   </si>
   <si>
     <t>Artist-Artist - Title (Artist - something Remix)</t>
+  </si>
+  <si>
+    <t>𝙁𝙍𝙀𝙀 𝘿𝙇_ Akon feat. Eminem - Smack That (Paranormila x SkaaR x E.B.A.H Edit)</t>
+  </si>
+  <si>
+    <t>$oho Bani - BLOCK THERAPIE (Techno Remix)</t>
+  </si>
+  <si>
+    <t>IN FURCHT - THREEFOLD SYMMETRY</t>
+  </si>
+  <si>
+    <t>DJ KINNƎR - CRAZY WIZARD SPELL</t>
+  </si>
+  <si>
+    <t>TBK - KEVIN (TRANCESTRUDEL EDIT)</t>
+  </si>
+  <si>
+    <t>RIANA HOLLEY &amp; SERAFINA - KIM POSSIBLE</t>
   </si>
 </sst>
 </file>
@@ -503,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28437CC-2DD0-43B3-B933-50C4FE5FA466}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,146 +539,176 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>